<commit_message>
Fixed so it doesn't prompt for input file location
commented out excessive code
</commit_message>
<xml_diff>
--- a/ForecastSummary.xlsx
+++ b/ForecastSummary.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$L$32</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
   <si>
     <t>ClassType</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Model_dynreg_auto.arima</t>
+  </si>
+  <si>
+    <t>e^-35</t>
   </si>
 </sst>
 </file>
@@ -192,8 +195,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -243,8 +246,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -547,10 +550,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L32"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -642,7 +646,7 @@
         <v>-0.53645770000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>31</v>
@@ -678,7 +682,7 @@
         <v>-0.20751459999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>31</v>
@@ -714,7 +718,7 @@
         <v>-8.8551740000000004E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>31</v>
@@ -750,7 +754,7 @@
         <v>-7.1080560000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>31</v>
@@ -786,7 +790,7 @@
         <v>-0.29132479999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>31</v>
@@ -822,7 +826,7 @@
         <v>1.3400820000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>31</v>
@@ -858,7 +862,7 @@
         <v>-4.8323960000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>31</v>
@@ -894,7 +898,7 @@
         <v>-9.1544760000000003E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
         <v>31</v>
@@ -930,7 +934,7 @@
         <v>-1.6038899999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>31</v>
@@ -966,7 +970,7 @@
         <v>5.2314399999999997E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>31</v>
@@ -1002,7 +1006,7 @@
         <v>3.9382619999999997E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
         <v>31</v>
@@ -1038,7 +1042,7 @@
         <v>1.7969269999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
         <v>31</v>
@@ -1074,7 +1078,7 @@
         <v>-3.5335039999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
         <v>31</v>
@@ -1110,7 +1114,7 @@
         <v>-3.5335039999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
         <v>31</v>
@@ -1146,7 +1150,7 @@
         <v>-4.9461060000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>31</v>
@@ -1182,7 +1186,7 @@
         <v>6.4505659999999996E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" t="s">
         <v>31</v>
@@ -1217,8 +1221,11 @@
       <c r="L18" s="3">
         <v>-4.006432E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" t="s">
         <v>31</v>
@@ -1254,7 +1261,7 @@
         <v>-6.7223770000000002E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" t="s">
         <v>31</v>
@@ -1290,7 +1297,7 @@
         <v>-2.6875550000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" t="s">
         <v>31</v>
@@ -1326,7 +1333,7 @@
         <v>-3.7924939999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" t="s">
         <v>31</v>
@@ -1362,7 +1369,7 @@
         <v>-0.25738559999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" t="s">
         <v>31</v>
@@ -1398,7 +1405,7 @@
         <v>0.2749878</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" t="s">
         <v>12</v>
@@ -1434,7 +1441,7 @@
         <v>-0.28190720000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" t="s">
         <v>27</v>
@@ -1470,7 +1477,7 @@
         <v>-0.28189969999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" t="s">
         <v>12</v>
@@ -1506,7 +1513,7 @@
         <v>-0.28189969999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" t="s">
         <v>12</v>
@@ -1542,7 +1549,7 @@
         <v>-0.35144209999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" t="s">
         <v>12</v>
@@ -1578,7 +1585,7 @@
         <v>2.384493E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" t="s">
         <v>12</v>
@@ -1614,7 +1621,7 @@
         <v>3.462672E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" t="s">
         <v>12</v>
@@ -1650,7 +1657,7 @@
         <v>3.3514189999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" t="s">
         <v>12</v>
@@ -1686,7 +1693,7 @@
         <v>2.918287E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" t="s">
         <v>12</v>
@@ -1723,7 +1730,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:L1">
+  <autoFilter ref="B1:L32">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="ets"/>
+        <filter val="forecast"/>
+      </filters>
+    </filterColumn>
     <sortState ref="B2:L32">
       <sortCondition ref="E1"/>
     </sortState>

</xml_diff>